<commit_message>
upload templates: updated column formats for dollar/mapping/hwsw/sales split upload templates, mostly the number columns to be numbers with 5 digit decimals
</commit_message>
<xml_diff>
--- a/database/files/prof/business-upload/dollar_upload_template.xlsx
+++ b/database/files/prof/business-upload/dollar_upload_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakahle\work\fin-dfa\database\files\business-upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dakahle\work\fin-dfa\database\files\prof\business-upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -456,24 +456,24 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6328125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -484,7 +484,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -495,13 +495,13 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -533,7 +533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -546,7 +546,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>